<commit_message>
jbcsep19 EJG 09/05/19 1st Push
</commit_message>
<xml_diff>
--- a/Wk1Challenge_ChooseYourOwnAdventure.xlsx
+++ b/Wk1Challenge_ChooseYourOwnAdventure.xlsx
@@ -9,11 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="3450"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$44</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$A:$A,Sheet1!$1:$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="325">
   <si>
     <r>
       <t>1.</t>
@@ -1853,6 +1857,12 @@
   </si>
   <si>
     <t>Variable</t>
+  </si>
+  <si>
+    <t>Map1</t>
+  </si>
+  <si>
+    <t>Map2</t>
   </si>
 </sst>
 </file>
@@ -2195,16 +2205,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:R44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="48.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="48.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="5" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="27.140625" bestFit="1" customWidth="1"/>
@@ -2217,8 +2231,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B1" t="s">
+        <v>323</v>
+      </c>
       <c r="C1" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="D1" t="s">
         <v>319</v>
@@ -4129,7 +4149,12 @@
       </c>
     </row>
   </sheetData>
+  <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="77" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;F</oddHeader>
+    <oddFooter>Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>